<commit_message>
Loss calculations are reviewed.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Conduction Loss</t>
   </si>
@@ -51,9 +51,6 @@
     <t>RDS</t>
   </si>
   <si>
-    <t>Irms</t>
-  </si>
-  <si>
     <t>Vdc</t>
   </si>
   <si>
@@ -108,13 +105,31 @@
     <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 20, Roff 2, Temp 150)</t>
   </si>
   <si>
-    <t>Enter Switching Energy Here</t>
+    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 10, Roff 2, Temp 150)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 10, Roff 2, Temp 25)</t>
+  </si>
+  <si>
+    <t>Ipeak</t>
+  </si>
+  <si>
+    <t>Enter Switching Energy Here for 25C</t>
+  </si>
+  <si>
+    <t>Enter Switching Energy Here for 150C</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 15, Roff 2, Temp 150)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,9 +162,109 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -159,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -169,7 +284,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -177,19 +291,46 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -472,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,26 +626,30 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -517,19 +662,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -544,15 +689,24 @@
         <v>5.1000000000000004E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>5.4</v>
-      </c>
-      <c r="E3" s="2">
-        <f>((POWER(B14,2)*C3*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C3*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D3*D14*E14/2))*C14</f>
-        <v>2.9238832428993495</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+        <v>5.7</v>
+      </c>
+      <c r="E3" s="26">
+        <f>(POWER(B14,2)*C3*0.25*(1-D14*E14))+B14*D3*D14*E14/(2*PI())</f>
+        <v>1.6625399895381963</v>
+      </c>
+      <c r="F3" s="26">
+        <f>(A19+C19)*D14*C14/PI()/2</f>
+        <v>3.0494087096407148</v>
+      </c>
+      <c r="G3" s="26">
+        <f>(B19+D19)*C14*D14/PI()/2</f>
+        <v>2.3554931577600509</v>
+      </c>
+      <c r="H3" s="26">
+        <f>SUM(E3:G3)</f>
+        <v>7.0674418569389612</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -567,15 +721,15 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>5.53</v>
-      </c>
-      <c r="E4" s="2">
-        <f>((POWER(B14,2)*C4*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C4*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D4*D14*E14/2))*C14</f>
-        <v>3.2586996913395194</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="E4" s="26">
+        <f>(POWER(B14,2)*C4*0.25*(1-D14*E14)+B14*D4*D14*E14/(2*PI()))</f>
+        <v>2.1418001256522161</v>
+      </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -589,15 +743,15 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="E5" s="2">
-        <f>((POWER(B14,2)*C5*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C5*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D5*D14*E14/2))*C14</f>
-        <v>3.5358958955456337</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+        <v>6.35</v>
+      </c>
+      <c r="E5" s="26">
+        <f>(POWER(B14,2)*C5*0.25*(1-D14*E14))++B14*D5*D14*E14/(2*PI())</f>
+        <v>2.6210602617662357</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -610,16 +764,16 @@
         <f t="shared" si="0"/>
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="D6" s="7">
-        <v>5.77</v>
-      </c>
-      <c r="E6" s="2">
-        <f>((POWER(B14,2)*C6*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C6*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D6*D14*E14/2))*C14</f>
-        <v>3.9787300576906013</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="D6" s="6">
+        <v>6.72</v>
+      </c>
+      <c r="E6" s="26">
+        <f>(POWER(B14,2)*C6*0.25*(1-D14*E14))+B14*D6*D14*E14/(2*PI())</f>
+        <v>3.1960285490345055</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -632,16 +786,16 @@
         <f t="shared" si="0"/>
         <v>0.11499999999999999</v>
       </c>
-      <c r="D7" s="7">
-        <v>5.9</v>
-      </c>
-      <c r="E7" s="2">
-        <f>((POWER(B14,2)*C7*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C7*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D7*D14*E14/2))*C14</f>
-        <v>4.3327465061307704</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10"/>
+      <c r="D7" s="6">
+        <v>7.11</v>
+      </c>
+      <c r="E7" s="26">
+        <f>(POWER(B14,2)*C7*0.25*(1-D14*E14))+B14*D7*D14*E14/(2*PI())</f>
+        <v>3.7075510923713288</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -655,46 +809,46 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="D8" s="2">
-        <v>6.02</v>
-      </c>
-      <c r="E8" s="2">
-        <f>((POWER(B14,2)*C8*(1/C14/2-G14/PI()/2/C14-D14*E14/2))+(POWER(B14,2)*C8*(G14/PI()/2/C14-D14*E14/2))+(B14*SQRT(2)/PI()*D8*D14*E14/2))*C14</f>
-        <v>4.7215616893063119</v>
-      </c>
-      <c r="F8" s="2">
-        <f>(A19+C19)*D14*C14/PI()/2</f>
-        <v>11.650141834326739</v>
-      </c>
-      <c r="G8" s="2">
-        <f>(B19+D19)*C14*D14/PI()/2</f>
-        <v>3.3196538030107532</v>
-      </c>
-      <c r="H8">
+        <v>7.56</v>
+      </c>
+      <c r="E8" s="26">
+        <f>(POWER(B14,2)*C8*0.25*(1-D14*E14))+B14*D8*D14*E14/(2*PI())</f>
+        <v>4.2830948839138179</v>
+      </c>
+      <c r="F8" s="26">
+        <f>(A22+C22)*D14*C14/PI()/2</f>
+        <v>9.9153529546250798</v>
+      </c>
+      <c r="G8" s="26">
+        <f>(B22+D22)*C14*D14/PI()/2</f>
+        <v>3.2117467515944478</v>
+      </c>
+      <c r="H8" s="30">
         <f>E8+F8+G8</f>
-        <v>19.691357326643804</v>
+        <v>17.410194590133344</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -702,18 +856,18 @@
         <v>270</v>
       </c>
       <c r="B14" s="2">
-        <v>8</v>
+        <v>11.3</v>
       </c>
       <c r="C14">
         <v>50</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>40000</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>0.9</v>
       </c>
       <c r="G14">
@@ -721,91 +875,278 @@
         <v>0.45102681179626236</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>29</v>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>4.0800000000000002E-5</v>
-      </c>
-      <c r="B19" s="5">
-        <v>5.1490000000000002E-6</v>
-      </c>
-      <c r="C19" s="5">
-        <v>-4.1999999999999996E-6</v>
-      </c>
-      <c r="D19" s="5">
-        <v>5.2800000000000003E-6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>28</v>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>1.3859999999999999E-5</v>
+      </c>
+      <c r="B19" s="20">
+        <v>4.9599999999999999E-6</v>
+      </c>
+      <c r="C19" s="20">
+        <v>-4.2799999999999997E-6</v>
+      </c>
+      <c r="D19" s="25">
+        <v>2.4399999999999999E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19">
+        <v>3.536E-5</v>
+      </c>
+      <c r="B22" s="20">
+        <v>5.31E-6</v>
+      </c>
+      <c r="C22" s="20">
+        <v>-4.2100000000000003E-6</v>
+      </c>
+      <c r="D22" s="20">
+        <v>4.78E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="I24" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="E25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="I25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="19">
         <v>4.0800000000000002E-5</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="20">
         <v>5.1490000000000002E-6</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="20">
         <v>-4.1999999999999996E-6</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="20">
         <v>5.2800000000000003E-6</v>
       </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="I26" s="19">
+        <v>3.536E-5</v>
+      </c>
+      <c r="J26" s="20">
+        <v>5.31E-6</v>
+      </c>
+      <c r="K26" s="20">
+        <v>-4.2100000000000003E-6</v>
+      </c>
+      <c r="L26" s="20">
+        <v>4.78E-6</v>
+      </c>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="24"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>2.9220000000000001E-5</v>
+      </c>
+      <c r="B30" s="20">
+        <v>5.1399999999999999E-6</v>
+      </c>
+      <c r="C30" s="20">
+        <v>-4.2300000000000002E-6</v>
+      </c>
+      <c r="D30" s="20">
+        <v>4.4900000000000002E-6</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>1.3859999999999999E-5</v>
+      </c>
+      <c r="B34" s="20">
+        <v>4.9599999999999999E-6</v>
+      </c>
+      <c r="C34" s="20">
+        <v>-4.2799999999999997E-6</v>
+      </c>
+      <c r="D34" s="20">
+        <v>2.4399999999999999E-6</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A24:D24"/>
+  <mergeCells count="12">
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="I24:O24"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="A20:D20"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A17:D17"/>

</xml_diff>

<commit_message>
Loss calculations are finalized with @mesutto
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -128,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -162,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -251,17 +251,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -294,7 +283,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,33 +315,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +605,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,17 +627,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -691,21 +680,21 @@
       <c r="D3" s="2">
         <v>5.7</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="19">
         <f>(POWER(B14,2)*C3*0.25*(1-D14*E14))+B14*D3*D14*E14/(2*PI())</f>
-        <v>1.6625399895381963</v>
-      </c>
-      <c r="F3" s="26">
-        <f>(A19+C19)*D14*C14/PI()/2</f>
-        <v>3.0494087096407148</v>
-      </c>
-      <c r="G3" s="26">
-        <f>(B19+D19)*C14*D14/PI()/2</f>
-        <v>2.3554931577600509</v>
-      </c>
-      <c r="H3" s="26">
+        <v>1.6711631119227452</v>
+      </c>
+      <c r="F3" s="19">
+        <f>(A19+C19)*D14/(PI()*2)</f>
+        <v>7.6235217741017866E-2</v>
+      </c>
+      <c r="G3" s="19">
+        <f>(B19+D19)*D14/PI()/2</f>
+        <v>5.8887328944001276E-2</v>
+      </c>
+      <c r="H3" s="19">
         <f>SUM(E3:G3)</f>
-        <v>7.0674418569389612</v>
+        <v>1.8062856586077645</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -723,13 +712,13 @@
       <c r="D4" s="2">
         <v>6.0250000000000004</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="19">
         <f>(POWER(B14,2)*C4*0.25*(1-D14*E14)+B14*D4*D14*E14/(2*PI()))</f>
-        <v>2.1418001256522161</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+        <v>2.15052890706527</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -745,13 +734,13 @@
       <c r="D5" s="2">
         <v>6.35</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="19">
         <f>(POWER(B14,2)*C5*0.25*(1-D14*E14))++B14*D5*D14*E14/(2*PI())</f>
-        <v>2.6210602617662357</v>
-      </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+        <v>2.6298947022077948</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -767,13 +756,13 @@
       <c r="D6" s="6">
         <v>6.72</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="19">
         <f>(POWER(B14,2)*C6*0.25*(1-D14*E14))+B14*D6*D14*E14/(2*PI())</f>
-        <v>3.1960285490345055</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+        <v>3.2049538112931315</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -789,13 +778,13 @@
       <c r="D7" s="6">
         <v>7.11</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="19">
         <f>(POWER(B14,2)*C7*0.25*(1-D14*E14))+B14*D7*D14*E14/(2*PI())</f>
-        <v>3.7075510923713288</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+        <v>3.7166669904641609</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -811,21 +800,21 @@
       <c r="D8" s="2">
         <v>7.56</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="19">
         <f>(POWER(B14,2)*C8*0.25*(1-D14*E14))+B14*D8*D14*E14/(2*PI())</f>
-        <v>4.2830948839138179</v>
-      </c>
-      <c r="F8" s="26">
-        <f>(A22+C22)*D14*C14/PI()/2</f>
-        <v>9.9153529546250798</v>
-      </c>
-      <c r="G8" s="26">
-        <f>(B22+D22)*C14*D14/PI()/2</f>
-        <v>3.2117467515944478</v>
-      </c>
-      <c r="H8" s="30">
+        <v>4.2924454798922724</v>
+      </c>
+      <c r="F8" s="19">
+        <f>(A22+C22)*D14/PI()/2</f>
+        <v>0.29125354585816848</v>
+      </c>
+      <c r="G8" s="19">
+        <f>(B22+D22)*D14/PI()/2</f>
+        <v>8.2991345075268841E-2</v>
+      </c>
+      <c r="H8" s="23">
         <f>E8+F8+G8</f>
-        <v>17.410194590133344</v>
+        <v>4.6666903708257097</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -862,7 +851,7 @@
         <v>50</v>
       </c>
       <c r="D14" s="5">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="E14" s="8">
         <v>9.9999999999999995E-8</v>
@@ -877,16 +866,16 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -895,7 +884,7 @@
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="12"/>
@@ -903,29 +892,29 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="15">
         <v>1.3859999999999999E-5</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="16">
         <v>4.9599999999999999E-6</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="16">
         <v>-4.2799999999999997E-6</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="31">
         <v>2.4399999999999999E-6</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -934,47 +923,47 @@
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
-        <v>3.536E-5</v>
-      </c>
-      <c r="B22" s="20">
-        <v>5.31E-6</v>
-      </c>
-      <c r="C22" s="20">
-        <v>-4.2100000000000003E-6</v>
-      </c>
-      <c r="D22" s="20">
-        <v>4.78E-6</v>
+      <c r="A22" s="15">
+        <v>4.0800000000000002E-5</v>
+      </c>
+      <c r="B22" s="16">
+        <v>5.1490000000000002E-6</v>
+      </c>
+      <c r="C22" s="16">
+        <v>-4.1999999999999996E-6</v>
+      </c>
+      <c r="D22" s="16">
+        <v>5.2800000000000003E-6</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="I24" s="14" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="I24" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="16"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="28"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -986,12 +975,12 @@
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="I25" s="17" t="s">
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
+      <c r="I25" s="13" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -1003,58 +992,58 @@
       <c r="L25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="21" t="s">
+      <c r="M25" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="N25" s="21"/>
-      <c r="O25" s="22"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="25"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19">
+      <c r="A26" s="15">
         <v>4.0800000000000002E-5</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="16">
         <v>5.1490000000000002E-6</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="16">
         <v>-4.1999999999999996E-6</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="16">
         <v>5.2800000000000003E-6</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="I26" s="19">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="I26" s="15">
         <v>3.536E-5</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="16">
         <v>5.31E-6</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="16">
         <v>-4.2100000000000003E-6</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="16">
         <v>4.78E-6</v>
       </c>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="24"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="18"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1066,43 +1055,43 @@
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19">
+      <c r="A30" s="15">
         <v>2.9220000000000001E-5</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="16">
         <v>5.1399999999999999E-6</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="16">
         <v>-4.2300000000000002E-6</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="16">
         <v>4.4900000000000002E-6</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1114,43 +1103,43 @@
       <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19">
+      <c r="A34" s="15">
         <v>1.3859999999999999E-5</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" s="16">
         <v>4.9599999999999999E-6</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="16">
         <v>-4.2799999999999997E-6</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="16">
         <v>2.4399999999999999E-6</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="I24:O24"/>
     <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:G6 H2">
     <cfRule type="dataBar" priority="3">

</xml_diff>

<commit_message>
Simulation analysis is done on GaN switching characteristics. It is seen that the mutual inductance between the power loop and the gate loop may affect the miller plateu even may deactivate the channel for short amount of time. This may explain the second pulse problem on gate source voltage false turn-on spike. Moreover, based on the recommendations, a new DPT code is created for chopper pulse test. Here, the voltage across the drain and source of a GaN will be followed to see whether the power loop bypass capacitors are capable of handling oscillations which emerge from repetitive switching. This problem, if exists, can be solved adding extra bypass capacitors.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Conduction Loss</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 15, Roff 2, Temp 150)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 270, Isw 22.6A, Ron 10, Roff 2, Temp 150)</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -300,6 +303,7 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,7 +325,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z34" sqref="Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,17 +631,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="29"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -682,19 +686,19 @@
       </c>
       <c r="E3" s="19">
         <f>(POWER(B14,2)*C3*0.25*(1-D14*E14))+B14*D3*D14*E14/(2*PI())</f>
-        <v>1.6711631119227452</v>
+        <v>2.4041285146094085</v>
       </c>
       <c r="F3" s="19">
         <f>(A19+C19)*D14/(PI()*2)</f>
-        <v>7.6235217741017866E-2</v>
+        <v>1.3722339193383217</v>
       </c>
       <c r="G3" s="19">
         <f>(B19+D19)*D14/PI()/2</f>
-        <v>5.8887328944001276E-2</v>
+        <v>1.0599719209920231</v>
       </c>
       <c r="H3" s="19">
         <f>SUM(E3:G3)</f>
-        <v>1.8062856586077645</v>
+        <v>4.8363343549397531</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -714,7 +718,7 @@
       </c>
       <c r="E4" s="19">
         <f>(POWER(B14,2)*C4*0.25*(1-D14*E14)+B14*D4*D14*E14/(2*PI()))</f>
-        <v>2.15052890706527</v>
+        <v>2.8924753271748571</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -736,7 +740,7 @@
       </c>
       <c r="E5" s="19">
         <f>(POWER(B14,2)*C5*0.25*(1-D14*E14))++B14*D5*D14*E14/(2*PI())</f>
-        <v>2.6298947022077948</v>
+        <v>3.3808221397403053</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="19"/>
@@ -758,7 +762,7 @@
       </c>
       <c r="E6" s="19">
         <f>(POWER(B14,2)*C6*0.25*(1-D14*E14))+B14*D6*D14*E14/(2*PI())</f>
-        <v>3.2049538112931315</v>
+        <v>3.9636011032763552</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -780,7 +784,7 @@
       </c>
       <c r="E7" s="19">
         <f>(POWER(B14,2)*C7*0.25*(1-D14*E14))+B14*D7*D14*E14/(2*PI())</f>
-        <v>3.7166669904641609</v>
+        <v>4.4915183283548927</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -802,19 +806,19 @@
       </c>
       <c r="E8" s="19">
         <f>(POWER(B14,2)*C8*0.25*(1-D14*E14))+B14*D8*D14*E14/(2*PI())</f>
-        <v>4.2924454798922724</v>
+        <v>5.0872461380609</v>
       </c>
       <c r="F8" s="19">
         <f>(A22+C22)*D14/PI()/2</f>
-        <v>0.29125354585816848</v>
+        <v>14.600468634145594</v>
       </c>
       <c r="G8" s="19">
         <f>(B22+D22)*D14/PI()/2</f>
-        <v>8.2991345075268841E-2</v>
+        <v>1.8058913505279635</v>
       </c>
       <c r="H8" s="23">
         <f>E8+F8+G8</f>
-        <v>4.6666903708257097</v>
+        <v>21.493606122734459</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -850,8 +854,8 @@
       <c r="C14">
         <v>50</v>
       </c>
-      <c r="D14" s="5">
-        <v>50000</v>
+      <c r="D14" s="32">
+        <v>900000</v>
       </c>
       <c r="E14" s="8">
         <v>9.9999999999999995E-8</v>
@@ -866,12 +870,12 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -901,17 +905,17 @@
       <c r="C19" s="16">
         <v>-4.2799999999999997E-6</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="24">
         <v>2.4399999999999999E-6</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -929,38 +933,38 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
-        <v>4.0800000000000002E-5</v>
+        <v>1.0609E-4</v>
       </c>
       <c r="B22" s="16">
-        <v>5.1490000000000002E-6</v>
+        <v>8.8179999999999993E-6</v>
       </c>
       <c r="C22" s="16">
-        <v>-4.1999999999999996E-6</v>
+        <v>-4.1594999999999997E-6</v>
       </c>
       <c r="D22" s="16">
-        <v>5.2800000000000003E-6</v>
+        <v>3.7894999999999999E-6</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="I24" s="26" t="s">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="I24" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -975,11 +979,11 @@
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
       <c r="I25" s="13" t="s">
         <v>17</v>
       </c>
@@ -992,11 +996,11 @@
       <c r="L25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="24" t="s">
+      <c r="M25" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N25" s="24"/>
-      <c r="O25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="26"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
@@ -1032,15 +1036,24 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="I28" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
@@ -1055,11 +1068,28 @@
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
+      <c r="I29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="25"/>
+      <c r="O29" s="26"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
@@ -1077,18 +1107,33 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
+      <c r="I30" s="15">
+        <v>1.0609E-4</v>
+      </c>
+      <c r="J30" s="16">
+        <v>8.8179999999999993E-6</v>
+      </c>
+      <c r="K30" s="16">
+        <v>-4.1594999999999997E-6</v>
+      </c>
+      <c r="L30" s="16">
+        <v>3.7894999999999999E-6</v>
+      </c>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="18"/>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -1103,11 +1148,11 @@
       <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
@@ -1127,7 +1172,7 @@
       <c r="G34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="E25:G25"/>
@@ -1140,6 +1185,8 @@
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="I24:O24"/>
     <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I28:O28"/>
+    <mergeCell ref="M29:O29"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:G6 H2">
     <cfRule type="dataBar" priority="3">

</xml_diff>

<commit_message>
Harmonic analysis for three phase inverter at 40 kHz and 10 kHz switching frequencies.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,6 +304,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,7 +326,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,17 +631,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -686,19 +686,19 @@
       </c>
       <c r="E3" s="19">
         <f>(POWER(B14,2)*C3*0.25*(1-D14*E14))+B14*D3*D14*E14/(2*PI())</f>
-        <v>2.4041285146094085</v>
+        <v>1.6625399895381963</v>
       </c>
       <c r="F3" s="19">
         <f>(A19+C19)*D14/(PI()*2)</f>
-        <v>1.3722339193383217</v>
+        <v>6.0988174192814291E-2</v>
       </c>
       <c r="G3" s="19">
         <f>(B19+D19)*D14/PI()/2</f>
-        <v>1.0599719209920231</v>
+        <v>4.7109863155201021E-2</v>
       </c>
       <c r="H3" s="19">
         <f>SUM(E3:G3)</f>
-        <v>4.8363343549397531</v>
+        <v>1.7706380268862114</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="E4" s="19">
         <f>(POWER(B14,2)*C4*0.25*(1-D14*E14)+B14*D4*D14*E14/(2*PI()))</f>
-        <v>2.8924753271748571</v>
+        <v>2.1418001256522161</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -740,7 +740,7 @@
       </c>
       <c r="E5" s="19">
         <f>(POWER(B14,2)*C5*0.25*(1-D14*E14))++B14*D5*D14*E14/(2*PI())</f>
-        <v>3.3808221397403053</v>
+        <v>2.6210602617662357</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="19"/>
@@ -762,7 +762,7 @@
       </c>
       <c r="E6" s="19">
         <f>(POWER(B14,2)*C6*0.25*(1-D14*E14))+B14*D6*D14*E14/(2*PI())</f>
-        <v>3.9636011032763552</v>
+        <v>3.1960285490345055</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -784,7 +784,7 @@
       </c>
       <c r="E7" s="19">
         <f>(POWER(B14,2)*C7*0.25*(1-D14*E14))+B14*D7*D14*E14/(2*PI())</f>
-        <v>4.4915183283548927</v>
+        <v>3.7075510923713288</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -806,19 +806,19 @@
       </c>
       <c r="E8" s="19">
         <f>(POWER(B14,2)*C8*0.25*(1-D14*E14))+B14*D8*D14*E14/(2*PI())</f>
-        <v>5.0872461380609</v>
+        <v>4.2830948839138179</v>
       </c>
       <c r="F8" s="19">
         <f>(A22+C22)*D14/PI()/2</f>
-        <v>14.600468634145594</v>
+        <v>0.6489097170731376</v>
       </c>
       <c r="G8" s="19">
         <f>(B22+D22)*D14/PI()/2</f>
-        <v>1.8058913505279635</v>
+        <v>8.0261837801242811E-2</v>
       </c>
       <c r="H8" s="23">
         <f>E8+F8+G8</f>
-        <v>21.493606122734459</v>
+        <v>5.0122664387881981</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -854,8 +854,8 @@
       <c r="C14">
         <v>50</v>
       </c>
-      <c r="D14" s="32">
-        <v>900000</v>
+      <c r="D14" s="25">
+        <v>40000</v>
       </c>
       <c r="E14" s="8">
         <v>9.9999999999999995E-8</v>
@@ -870,12 +870,12 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -910,12 +910,12 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -947,24 +947,24 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
-      <c r="I24" s="27" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
+      <c r="I24" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="30"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -979,11 +979,11 @@
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
       <c r="I25" s="13" t="s">
         <v>17</v>
       </c>
@@ -996,11 +996,11 @@
       <c r="L25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="25" t="s">
+      <c r="M25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="N25" s="25"/>
-      <c r="O25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
@@ -1036,24 +1036,24 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="I28" s="27" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30"/>
+      <c r="I28" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="30"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
@@ -1068,11 +1068,11 @@
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
       <c r="I29" s="13" t="s">
         <v>17</v>
       </c>
@@ -1085,11 +1085,11 @@
       <c r="L29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="25" t="s">
+      <c r="M29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="N29" s="25"/>
-      <c r="O29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="27"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
@@ -1125,15 +1125,15 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
@@ -1148,11 +1148,11 @@
       <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
@@ -1173,12 +1173,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A28:G28"/>
@@ -1187,6 +1181,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="I28:O28"/>
     <mergeCell ref="M29:O29"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:G6 H2">
     <cfRule type="dataBar" priority="3">

</xml_diff>

<commit_message>
A few parts of the article is completed. The parasitics of each bypass and film capacitor connections are extracted using Q3D. These values are implemented in LT Spice model to find switching energies. The switching energies are obtained for 300V, 2:2:12 Apeak at 110C junction temperature. These results are given in the article.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>Conduction Loss</t>
   </si>
@@ -102,28 +102,40 @@
     <t>Pcond</t>
   </si>
   <si>
-    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 20, Roff 2, Temp 150)</t>
-  </si>
-  <si>
-    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 10, Roff 2, Temp 150)</t>
-  </si>
-  <si>
-    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 10, Roff 2, Temp 25)</t>
-  </si>
-  <si>
     <t>Ipeak</t>
   </si>
   <si>
-    <t>Enter Switching Energy Here for 25C</t>
-  </si>
-  <si>
-    <t>Enter Switching Energy Here for 150C</t>
-  </si>
-  <si>
-    <t>Switching Energy (Vdc 270, Isw 11.3A, Ron 15, Roff 2, Temp 150)</t>
-  </si>
-  <si>
-    <t>Switching Energy (Vdc 270, Isw 22.6A, Ron 10, Roff 2, Temp 150)</t>
+    <t>110C</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 11A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 2A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 4A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 6A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 8A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 10A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 12A, Ron 22, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Enter Switching Energy Here for 110C</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 11A, Ron 16, Roff 2, Temp 110)</t>
+  </si>
+  <si>
+    <t>Switching Energy (Vdc 300, Isw 11A, Ron 10, Roff 2, Temp 110)</t>
   </si>
 </sst>
 </file>
@@ -266,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -303,7 +315,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +337,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +636,8 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
@@ -628,20 +646,24 @@
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -678,27 +700,27 @@
         <v>0.51</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C8" si="0">B3/10</f>
+        <f t="shared" ref="C3:C9" si="0">B3/10</f>
         <v>5.1000000000000004E-2</v>
       </c>
       <c r="D3" s="2">
         <v>5.7</v>
       </c>
       <c r="E3" s="19">
-        <f>(POWER(B14,2)*C3*0.25*(1-D14*E14))+B14*D3*D14*E14/(2*PI())</f>
-        <v>1.6625399895381963</v>
-      </c>
-      <c r="F3" s="19">
-        <f>(A19+C19)*D14/(PI()*2)</f>
-        <v>6.0988174192814291E-2</v>
-      </c>
-      <c r="G3" s="19">
-        <f>(B19+D19)*D14/PI()/2</f>
-        <v>4.7109863155201021E-2</v>
-      </c>
-      <c r="H3" s="19">
+        <f>(POWER(B15,2)*C3*0.25*(1-D15*E15))+B15*D3*D15*E15/(2*PI())</f>
+        <v>1.5764950597274474</v>
+      </c>
+      <c r="F3" s="19" t="e">
+        <f>(#REF!+#REF!)*D15/(PI()*2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G3" s="19" t="e">
+        <f>(#REF!+#REF!)*D15/PI()/2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H3" s="19" t="e">
         <f>SUM(E3:G3)</f>
-        <v>1.7706380268862114</v>
+        <v>#REF!</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -717,8 +739,8 @@
         <v>6.0250000000000004</v>
       </c>
       <c r="E4" s="19">
-        <f>(POWER(B14,2)*C4*0.25*(1-D14*E14)+B14*D4*D14*E14/(2*PI()))</f>
-        <v>2.1418001256522161</v>
+        <f>(POWER(B15,2)*C4*0.25*(1-D15*E15)+B15*D4*D15*E15/(2*PI()))</f>
+        <v>2.0307059754136616</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -739,8 +761,8 @@
         <v>6.35</v>
       </c>
       <c r="E5" s="19">
-        <f>(POWER(B14,2)*C5*0.25*(1-D14*E14))++B14*D5*D14*E14/(2*PI())</f>
-        <v>2.6210602617662357</v>
+        <f>(POWER(B15,2)*C5*0.25*(1-D15*E15))++B15*D5*D15*E15/(2*PI())</f>
+        <v>2.4849168910998758</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="19"/>
@@ -761,434 +783,725 @@
         <v>6.72</v>
       </c>
       <c r="E6" s="19">
-        <f>(POWER(B14,2)*C6*0.25*(1-D14*E14))+B14*D6*D14*E14/(2*PI())</f>
-        <v>3.1960285490345055</v>
+        <f>(POWER(B15,2)*C6*0.25*(1-D15*E15))+B15*D6*D15*E15/(2*PI())</f>
+        <v>3.0298299335734118</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="D7" s="32">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="19">
+        <f>(POWER(B15,2)*C7*0.25*(1-D15*E15))+B15*D7*D15*E15/(2*PI())</f>
+        <v>3.5082524684754692</v>
+      </c>
+      <c r="F7" s="19">
+        <f>(A20+C20)*D15/(PI()*2)</f>
+        <v>0.16934085944977664</v>
+      </c>
+      <c r="G7" s="19">
+        <f>(B20+D20)*D15/PI()/2</f>
+        <v>6.6463104235175499E-2</v>
+      </c>
+      <c r="H7" s="19">
+        <f>SUM(E7:G7)</f>
+        <v>3.7440564321604213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>0.11499999999999999</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="6">
         <v>7.11</v>
       </c>
-      <c r="E7" s="19">
-        <f>(POWER(B14,2)*C7*0.25*(1-D14*E14))+B14*D7*D14*E14/(2*PI())</f>
-        <v>3.7075510923713288</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="E8" s="19">
+        <f>(POWER(B15,2)*C8*0.25*(1-D15*E15))+B15*D8*D15*E15/(2*PI())</f>
+        <v>3.5146250323968684</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>1.33</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>0.13300000000000001</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>7.56</v>
       </c>
-      <c r="E8" s="19">
-        <f>(POWER(B14,2)*C8*0.25*(1-D14*E14))+B14*D8*D14*E14/(2*PI())</f>
-        <v>4.2830948839138179</v>
-      </c>
-      <c r="F8" s="19">
-        <f>(A22+C22)*D14/PI()/2</f>
-        <v>0.6489097170731376</v>
-      </c>
-      <c r="G8" s="19">
-        <f>(B22+D22)*D14/PI()/2</f>
-        <v>8.0261837801242811E-2</v>
-      </c>
-      <c r="H8" s="23">
-        <f>E8+F8+G8</f>
-        <v>5.0122664387881981</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="E9" s="19">
+        <f>(POWER(B15,2)*C9*0.25*(1-D15*E15))+B15*D9*D15*E15/(2*PI())</f>
+        <v>4.0600983002700888</v>
+      </c>
+      <c r="F9" s="19">
+        <f>(A23+C23)*D15/PI()/2</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <f>(B23+D23)*D15/PI()/2</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <f>E9+F9+G9</f>
+        <v>4.0600983002700888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>300</v>
+      </c>
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15" s="24">
+        <v>40000</v>
+      </c>
+      <c r="E15" s="8">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G15">
+        <f>ACOS(F15)</f>
+        <v>0.45102681179626236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="G19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>270</v>
-      </c>
-      <c r="B14" s="2">
-        <v>11.3</v>
-      </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-      <c r="D14" s="25">
-        <v>40000</v>
-      </c>
-      <c r="E14" s="8">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="G14">
-        <f>ACOS(F14)</f>
-        <v>0.45102681179626236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>3.1510000000000002E-5</v>
+      </c>
+      <c r="B20" s="16">
+        <v>5.4199999999999998E-6</v>
+      </c>
+      <c r="C20" s="16">
+        <v>-4.9100000000000004E-6</v>
+      </c>
+      <c r="D20" s="16">
+        <v>5.0200000000000002E-6</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="G21" s="15">
+        <v>1.5569999999999998E-5</v>
+      </c>
+      <c r="H21" s="16">
+        <v>4.9300000000000002E-6</v>
+      </c>
+      <c r="I21" s="16">
+        <v>-4.7999999999999998E-6</v>
+      </c>
+      <c r="J21" s="16">
+        <v>5.0200000000000002E-6</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="G22" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="G23" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="J23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
-        <v>1.3859999999999999E-5</v>
-      </c>
-      <c r="B19" s="16">
-        <v>4.9599999999999999E-6</v>
-      </c>
-      <c r="C19" s="16">
-        <v>-4.2799999999999997E-6</v>
-      </c>
-      <c r="D19" s="24">
-        <v>2.4399999999999999E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="K23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="15">
+        <v>2.0040000000000001E-5</v>
+      </c>
+      <c r="H24" s="16">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="I24" s="16">
+        <v>-4.5900000000000001E-6</v>
+      </c>
+      <c r="J24" s="16">
+        <v>4.9799999999999998E-6</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="J26" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
-        <v>1.0609E-4</v>
-      </c>
-      <c r="B22" s="16">
-        <v>8.8179999999999993E-6</v>
-      </c>
-      <c r="C22" s="16">
-        <v>-4.1594999999999997E-6</v>
-      </c>
-      <c r="D22" s="16">
-        <v>3.7894999999999999E-6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
-      <c r="I24" s="28" t="s">
+      <c r="K26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="25"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="15">
+        <v>2.5320000000000002E-5</v>
+      </c>
+      <c r="H27" s="16">
+        <v>5.0100000000000003E-6</v>
+      </c>
+      <c r="I27" s="16">
+        <v>-4.8300000000000003E-6</v>
+      </c>
+      <c r="J27" s="16">
+        <v>4.8600000000000001E-6</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="30"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="J29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="K29" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="I25" s="13" t="s">
+      <c r="L29" s="25"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="15">
+        <v>3.1279999999999999E-5</v>
+      </c>
+      <c r="H30" s="16">
+        <v>5.0200000000000002E-6</v>
+      </c>
+      <c r="I30" s="16">
+        <v>-4.7099999999999998E-6</v>
+      </c>
+      <c r="J30" s="16">
+        <v>4.8500000000000002E-6</v>
+      </c>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="26" t="s">
+      <c r="K32" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N25" s="26"/>
-      <c r="O25" s="27"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
-        <v>4.0800000000000002E-5</v>
-      </c>
-      <c r="B26" s="16">
-        <v>5.1490000000000002E-6</v>
-      </c>
-      <c r="C26" s="16">
-        <v>-4.1999999999999996E-6</v>
-      </c>
-      <c r="D26" s="16">
-        <v>5.2800000000000003E-6</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="I26" s="15">
-        <v>3.536E-5</v>
-      </c>
-      <c r="J26" s="16">
-        <v>5.31E-6</v>
-      </c>
-      <c r="K26" s="16">
-        <v>-4.2100000000000003E-6</v>
-      </c>
-      <c r="L26" s="16">
-        <v>4.78E-6</v>
-      </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="18"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
-      <c r="I28" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="30"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="L32" s="25"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="15">
+        <v>3.8819999999999998E-5</v>
+      </c>
+      <c r="H33" s="16">
+        <v>5.0699999999999997E-6</v>
+      </c>
+      <c r="I33" s="16">
+        <v>-4.9100000000000004E-6</v>
+      </c>
+      <c r="J33" s="16">
+        <v>4.9400000000000001E-6</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="28"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="28"/>
+      <c r="AA34" s="29"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="H35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="K35" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="I29" s="13" t="s">
+      <c r="L35" s="25"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="O35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="P35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="Q35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="26" t="s">
+      <c r="R35" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N29" s="26"/>
-      <c r="O29" s="27"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15">
-        <v>2.9220000000000001E-5</v>
-      </c>
-      <c r="B30" s="16">
-        <v>5.1399999999999999E-6</v>
-      </c>
-      <c r="C30" s="16">
-        <v>-4.2300000000000002E-6</v>
-      </c>
-      <c r="D30" s="16">
-        <v>4.4900000000000002E-6</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="15">
-        <v>1.0609E-4</v>
-      </c>
-      <c r="J30" s="16">
-        <v>8.8179999999999993E-6</v>
-      </c>
-      <c r="K30" s="16">
-        <v>-4.1594999999999997E-6</v>
-      </c>
-      <c r="L30" s="16">
-        <v>3.7894999999999999E-6</v>
-      </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="18"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="S35" s="25"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="V35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="W35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="X35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="Y35" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
-        <v>1.3859999999999999E-5</v>
-      </c>
-      <c r="B34" s="16">
-        <v>4.9599999999999999E-6</v>
-      </c>
-      <c r="C34" s="16">
-        <v>-4.2799999999999997E-6</v>
-      </c>
-      <c r="D34" s="16">
-        <v>2.4399999999999999E-6</v>
-      </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="26"/>
+    </row>
+    <row r="36" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="15">
+        <v>4.2500000000000003E-5</v>
+      </c>
+      <c r="H36" s="16">
+        <v>5.4199999999999998E-6</v>
+      </c>
+      <c r="I36" s="16">
+        <v>-4.7999999999999998E-6</v>
+      </c>
+      <c r="J36" s="16">
+        <v>5.1900000000000003E-6</v>
+      </c>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="15">
+        <v>3.68E-5</v>
+      </c>
+      <c r="O36" s="16">
+        <v>5.2700000000000004E-6</v>
+      </c>
+      <c r="P36" s="16">
+        <v>-4.9200000000000003E-6</v>
+      </c>
+      <c r="Q36" s="16">
+        <v>4.95E-6</v>
+      </c>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="18"/>
+      <c r="U36" s="15">
+        <v>3.1510000000000002E-5</v>
+      </c>
+      <c r="V36" s="16">
+        <v>5.4199999999999998E-6</v>
+      </c>
+      <c r="W36" s="16">
+        <v>-4.9100000000000004E-6</v>
+      </c>
+      <c r="X36" s="16">
+        <v>5.0200000000000002E-6</v>
+      </c>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="18"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G37" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="29"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="25"/>
+      <c r="M38" s="26"/>
+    </row>
+    <row r="39" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="15">
+        <v>4.6999999999999997E-5</v>
+      </c>
+      <c r="H39" s="16">
+        <v>5.4500000000000003E-6</v>
+      </c>
+      <c r="I39" s="16">
+        <v>-4.8099999999999997E-6</v>
+      </c>
+      <c r="J39" s="16">
+        <v>4.7999999999999998E-6</v>
+      </c>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="I24:O24"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I28:O28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="E25:G25"/>
+  <mergeCells count="22">
+    <mergeCell ref="N34:T34"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="U34:AA34"/>
+    <mergeCell ref="Y35:AA35"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="G37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="G28:M28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="G31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="G22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="G19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="G25:M25"/>
+    <mergeCell ref="A21:D21"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A17:D17"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:G6 H2">
+  <conditionalFormatting sqref="F2:G7 H2">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1202,7 +1515,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:E8">
+  <conditionalFormatting sqref="A3:E6 A8:E9 B7:E7">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1216,7 +1529,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:H8">
+  <conditionalFormatting sqref="E3:H9">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1246,7 +1559,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:G6 H2</xm:sqref>
+          <xm:sqref>F2:G7 H2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{221A22F0-197A-4E51-B8F8-E3F592256288}">
@@ -1259,7 +1572,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A3:E8</xm:sqref>
+          <xm:sqref>A3:E6 A8:E9 B7:E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{81E0BBFF-1C6F-4619-9AE2-21C98DB3EFE2}">
@@ -1272,7 +1585,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E3:H8</xm:sqref>
+          <xm:sqref>E3:H9</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Düşük güçler için kalorimetre testleri yapıldı. 2 kademede düzgün sonuç alınamadı. 1. kademe yapılmadı. Loss düzeltmeleri yapıldı, makaleye işlenecek. Termal analiz tıkandı, tekrar bakılacak. @furkankarakaya, @ozank
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
+++ b/Project/3501/Furkan/Loss LTSpice/Loss Analytical.xlsx
@@ -423,7 +423,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -482,19 +482,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2988842918755457</c:v>
+                  <c:v>2.0823085837510913</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.057558565380345</c:v>
+                  <c:v>3.99338963076069</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.084196152993238</c:v>
+                  <c:v>7.2224723059864733</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.8209124421679</c:v>
+                  <c:v>12.213199884335802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.157763071734522</c:v>
+                  <c:v>19.914833643469045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,7 +559,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="99425600"/>
@@ -618,7 +618,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="tr-TR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2089170672"/>
@@ -659,7 +659,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="tr-TR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,28 +1616,28 @@
         <v>8.591E-2</v>
       </c>
       <c r="E3" s="19">
-        <f>(H11+J11)*E11/(PI()*2)</f>
-        <v>6.6908738075832808E-2</v>
+        <f>(H11+J11)*E11/(PI())</f>
+        <v>0.13381747615166562</v>
       </c>
       <c r="F3" s="19">
-        <f>(I11+K11)*E11/PI()/2</f>
-        <v>6.3661977236758135E-2</v>
+        <f>(I11+K11)*E11/PI()</f>
+        <v>0.12732395447351627</v>
       </c>
       <c r="G3" s="19">
         <f>SUM(D3:F3)</f>
-        <v>0.21648071531259094</v>
+        <v>0.34705143062518184</v>
       </c>
       <c r="H3" s="2">
         <f>6*G3</f>
-        <v>1.2988842918755457</v>
+        <v>2.0823085837510913</v>
       </c>
       <c r="I3">
         <f>6*(G3-D3)</f>
-        <v>0.78342429187554574</v>
+        <v>1.5668485837510913</v>
       </c>
       <c r="J3">
         <f>H3-I3</f>
-        <v>0.51545999999999992</v>
+        <v>0.51546000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1656,24 +1656,24 @@
         <v>0.35362125000000005</v>
       </c>
       <c r="E4" s="19">
-        <f t="shared" ref="E4:E5" si="0">(H12+J12)*E12/(PI()*2)</f>
-        <v>9.3010148742903642E-2</v>
+        <f t="shared" ref="E4:E7" si="0">(H12+J12)*E12/(PI())</f>
+        <v>0.18602029748580728</v>
       </c>
       <c r="F4" s="19">
-        <f t="shared" ref="F4:F7" si="1">(I12+K12)*E12/PI()/2</f>
-        <v>6.2961695487153801E-2</v>
+        <f t="shared" ref="F4:F7" si="1">(I12+K12)*E12/PI()</f>
+        <v>0.1259233909743076</v>
       </c>
       <c r="G4" s="19">
         <f t="shared" ref="G4:G7" si="2">SUM(D4:F4)</f>
-        <v>0.5095930942300575</v>
+        <v>0.665564938460115</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ref="H4:H7" si="3">6*G4</f>
-        <v>3.057558565380345</v>
+        <v>3.99338963076069</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I7" si="4">6*(G4-D4)</f>
-        <v>0.93583106538034466</v>
+        <v>1.8716621307606895</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J7" si="5">H4-I4</f>
@@ -1697,23 +1697,23 @@
       </c>
       <c r="E5" s="19">
         <f t="shared" si="0"/>
-        <v>0.12605071492878112</v>
+        <v>0.25210142985756223</v>
       </c>
       <c r="F5" s="19">
         <f t="shared" si="1"/>
-        <v>6.3661977236758135E-2</v>
+        <v>0.12732395447351627</v>
       </c>
       <c r="G5" s="19">
         <f t="shared" si="2"/>
-        <v>1.0140326921655396</v>
+        <v>1.2037453843310788</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="3"/>
-        <v>6.084196152993238</v>
+        <v>7.2224723059864733</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>1.1382761529932359</v>
+        <v>2.2765523059864714</v>
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
@@ -1736,24 +1736,24 @@
         <v>1.5714375</v>
       </c>
       <c r="E6" s="19">
-        <f>(H14+J14)*E14/(PI()*2)</f>
-        <v>0.16870423967740908</v>
+        <f t="shared" si="0"/>
+        <v>0.33740847935481816</v>
       </c>
       <c r="F6" s="19">
         <f t="shared" si="1"/>
-        <v>6.334366735057434E-2</v>
+        <v>0.12668733470114868</v>
       </c>
       <c r="G6" s="19">
         <f t="shared" si="2"/>
-        <v>1.8034854070279833</v>
+        <v>2.035533314055967</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="3"/>
-        <v>10.8209124421679</v>
+        <v>12.213199884335802</v>
       </c>
       <c r="I6">
         <f>6*(G6-D6)</f>
-        <v>1.3922874421678997</v>
+        <v>2.784574884335802</v>
       </c>
       <c r="J6">
         <f t="shared" si="5"/>
@@ -1776,24 +1776,24 @@
         <v>2.7334487499999995</v>
       </c>
       <c r="E7" s="19">
-        <f>(H15+J15)*E15/(PI()*2)</f>
-        <v>0.22848283630272492</v>
+        <f t="shared" si="0"/>
+        <v>0.45696567260544985</v>
       </c>
       <c r="F7" s="19">
         <f t="shared" si="1"/>
-        <v>6.4362258986362469E-2</v>
+        <v>0.12872451797272494</v>
       </c>
       <c r="G7" s="19">
         <f t="shared" si="2"/>
-        <v>3.0262938452890871</v>
+        <v>3.3191389405781742</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="3"/>
-        <v>18.157763071734522</v>
+        <v>19.914833643469045</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>1.7570705717345252</v>
+        <v>3.5141411434690477</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
@@ -2061,15 +2061,15 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10">
         <f>(I4-I3)/I3*100</f>
-        <v>19.453924914675756</v>
+        <v>19.453924914675788</v>
       </c>
       <c r="I19" s="10">
         <f>(J4-J3)/J3*100</f>
-        <v>311.6182632988012</v>
+        <v>311.61826329880114</v>
       </c>
       <c r="J19" s="10">
         <f>I3/C11</f>
-        <v>0.35610195085252078</v>
+        <v>0.71220390170504144</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2097,7 +2097,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="10">
         <f t="shared" ref="H20:I22" si="8">(I5-I4)/I4*100</f>
-        <v>21.632653061224531</v>
+        <v>21.632653061224492</v>
       </c>
       <c r="I20" s="10">
         <f t="shared" si="8"/>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="J20" s="10">
         <f t="shared" ref="J20:J22" si="9">I4/C12</f>
-        <v>0.21763513148380109</v>
+        <v>0.43527026296760224</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
@@ -2136,7 +2136,7 @@
       <c r="G21" s="26"/>
       <c r="H21" s="10">
         <f t="shared" si="8"/>
-        <v>22.315436241610623</v>
+        <v>22.315436241610765</v>
       </c>
       <c r="I21" s="10">
         <f t="shared" si="8"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="J21" s="10">
         <f t="shared" si="9"/>
-        <v>0.17785564890519309</v>
+        <v>0.35571129781038613</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -2175,7 +2175,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10">
         <f t="shared" si="8"/>
-        <v>26.20027434842261</v>
+        <v>26.200274348422393</v>
       </c>
       <c r="I22" s="10">
         <f t="shared" si="8"/>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="J22" s="10">
         <f t="shared" si="9"/>
-        <v>0.16379852260798819</v>
+        <v>0.32759704521597671</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -2732,7 +2732,7 @@
     <mergeCell ref="N34:T34"/>
     <mergeCell ref="U34:AA34"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:F7 G2:J2">
+  <conditionalFormatting sqref="G2:J2 E2:F7">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -2805,7 +2805,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E2:F7 G2:J2</xm:sqref>
+          <xm:sqref>G2:J2 E2:F7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{36B65837-8CFE-4DF8-BCC9-4C93D79B8D31}">
@@ -3709,12 +3709,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="N34:T34"/>
-    <mergeCell ref="R35:T35"/>
-    <mergeCell ref="U34:AA34"/>
-    <mergeCell ref="Y35:AA35"/>
-    <mergeCell ref="G34:M34"/>
-    <mergeCell ref="K35:M35"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="G37:M37"/>
@@ -3731,6 +3725,12 @@
     <mergeCell ref="K20:M20"/>
     <mergeCell ref="G25:M25"/>
     <mergeCell ref="A21:D21"/>
+    <mergeCell ref="N34:T34"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="U34:AA34"/>
+    <mergeCell ref="Y35:AA35"/>
+    <mergeCell ref="G34:M34"/>
+    <mergeCell ref="K35:M35"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:G7 H2">
     <cfRule type="dataBar" priority="3">

</xml_diff>